<commit_message>
chore: rename to Net_Revenue_EUR and Net_Revenue_Percentage
</commit_message>
<xml_diff>
--- a/merged_df.xlsx
+++ b/merged_df.xlsx
@@ -606,12 +606,12 @@
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>Bet_Profit_EUR</t>
+          <t>Net_Revenue_EUR</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>Bet_Profit_Percentage</t>
+          <t>Net_Revenue_Percentage</t>
         </is>
       </c>
     </row>

</xml_diff>